<commit_message>
Tidy up & reset for presentation
</commit_message>
<xml_diff>
--- a/JSizzle-Demo/doc/You.xlsx
+++ b/JSizzle-Demo/doc/You.xlsx
@@ -14,38 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Tool</t>
-  </si>
-  <si>
-    <t>UML</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>JSizzle</t>
-  </si>
-  <si>
-    <t>Number_Happy</t>
-  </si>
-  <si>
-    <t>Number_Unhappy</t>
-  </si>
-  <si>
-    <t>Spock</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>behaviour</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F9:J15"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,88 +363,7 @@
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="9" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>